<commit_message>
falta pseudocodi, pas a pas i intro i conclusions
</commit_message>
<xml_diff>
--- a/scripts/data/data.xlsx
+++ b/scripts/data/data.xlsx
@@ -471,22 +471,22 @@
         <v>125</v>
       </c>
       <c r="B2" t="n">
-        <v>0.022729171003447</v>
+        <v>0.0283232344</v>
       </c>
       <c r="C2" t="n">
-        <v>0.000992366003629</v>
+        <v>0.0006822424</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0005622939934250001</v>
+        <v>0.0004153632</v>
       </c>
       <c r="E2" t="n">
-        <v>0.000939213998208</v>
+        <v>0.0009877962000000001</v>
       </c>
       <c r="F2" t="n">
-        <v>0.000707084996975</v>
+        <v>0.0007164220000000001</v>
       </c>
       <c r="G2" t="n">
-        <v>0.001425973998266</v>
+        <v>0.000424609</v>
       </c>
     </row>
     <row r="3">
@@ -494,22 +494,22 @@
         <v>250</v>
       </c>
       <c r="B3" t="n">
-        <v>0.169327909999992</v>
+        <v>0.2121381092</v>
       </c>
       <c r="C3" t="n">
-        <v>0.003617374997702</v>
+        <v>0.0032709344</v>
       </c>
       <c r="D3" t="n">
-        <v>0.001596325993887</v>
+        <v>0.0008710728</v>
       </c>
       <c r="E3" t="n">
-        <v>0.002762616997642</v>
+        <v>0.0019942228</v>
       </c>
       <c r="F3" t="n">
-        <v>0.002773465996142</v>
+        <v>0.0027361546</v>
       </c>
       <c r="G3" t="n">
-        <v>0.005250366994005</v>
+        <v>0.0009780699999999999</v>
       </c>
     </row>
     <row r="4">
@@ -517,22 +517,22 @@
         <v>500</v>
       </c>
       <c r="B4" t="n">
-        <v>1.402152984999702</v>
+        <v>1.6764079678</v>
       </c>
       <c r="C4" t="n">
-        <v>0.015824885995243</v>
+        <v>0.013376783</v>
       </c>
       <c r="D4" t="n">
-        <v>0.002275139995617</v>
+        <v>0.0018909846</v>
       </c>
       <c r="E4" t="n">
-        <v>0.00331739399553</v>
+        <v>0.0074744184</v>
       </c>
       <c r="F4" t="n">
-        <v>0.01221011000598</v>
+        <v>0.0118008174</v>
       </c>
       <c r="G4" t="n">
-        <v>0.020021592004923</v>
+        <v>0.0024347038</v>
       </c>
     </row>
     <row r="5">
@@ -540,22 +540,22 @@
         <v>1000</v>
       </c>
       <c r="B5" t="n">
-        <v>12.06846092300111</v>
+        <v>14.0336218528</v>
       </c>
       <c r="C5" t="n">
-        <v>0.058930047998728</v>
+        <v>0.0517733154</v>
       </c>
       <c r="D5" t="n">
-        <v>0.004325491994677</v>
+        <v>0.0041477716</v>
       </c>
       <c r="E5" t="n">
-        <v>0.019644342995889</v>
+        <v>0.0372150808</v>
       </c>
       <c r="F5" t="n">
-        <v>0.046189114000299</v>
+        <v>0.05080168500000001</v>
       </c>
       <c r="G5" t="n">
-        <v>0.07168005699350001</v>
+        <v>0.0060820926</v>
       </c>
     </row>
     <row r="6">
@@ -563,22 +563,22 @@
         <v>2000</v>
       </c>
       <c r="B6" t="n">
-        <v>98.32347272399784</v>
+        <v>116.941428585</v>
       </c>
       <c r="C6" t="n">
-        <v>0.241624993999721</v>
+        <v>0.1998502272</v>
       </c>
       <c r="D6" t="n">
-        <v>0.010494421003386</v>
+        <v>0.0094201748</v>
       </c>
       <c r="E6" t="n">
-        <v>0.09612536600616201</v>
+        <v>0.109190961</v>
       </c>
       <c r="F6" t="n">
-        <v>0.171501519005687</v>
+        <v>0.1903564716</v>
       </c>
       <c r="G6" t="n">
-        <v>0.269174606000888</v>
+        <v>0.0131280356</v>
       </c>
     </row>
     <row r="7">
@@ -586,22 +586,22 @@
         <v>4000</v>
       </c>
       <c r="B7" t="n">
-        <v>836.966712584006</v>
+        <v>966.9290217122</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9480921480062531</v>
+        <v>0.8066466206</v>
       </c>
       <c r="D7" t="n">
-        <v>0.024334297995665</v>
+        <v>0.0207859002</v>
       </c>
       <c r="E7" t="n">
-        <v>0.179570149004575</v>
+        <v>0.3700318532</v>
       </c>
       <c r="F7" t="n">
-        <v>0.64731833100086</v>
+        <v>0.7497630564000001</v>
       </c>
       <c r="G7" t="n">
-        <v>1.059995265000907</v>
+        <v>0.028741423</v>
       </c>
     </row>
     <row r="8">
@@ -610,19 +610,19 @@
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="n">
-        <v>3.817473811002855</v>
+        <v>3.2098342538</v>
       </c>
       <c r="D8" t="n">
-        <v>0.04769779399794</v>
+        <v>0.0450456594</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9994135140004801</v>
+        <v>1.5996798728</v>
       </c>
       <c r="F8" t="n">
-        <v>2.641624399999273</v>
+        <v>2.9972841358</v>
       </c>
       <c r="G8" t="n">
-        <v>4.306255552000948</v>
+        <v>0.0644687556</v>
       </c>
     </row>
   </sheetData>

</xml_diff>